<commit_message>
season bounds now set with Excel
</commit_message>
<xml_diff>
--- a/MATLAB_code/seasons_wKLedits.2024.07.03.xlsx
+++ b/MATLAB_code/seasons_wKLedits.2024.07.03.xlsx
@@ -8,59 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\GitHub\BATSallTime\MATLAB_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49024F3-890C-4F0D-9BEC-DD79FF8BD79D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDB435B-47D7-421A-83FC-F2DCA3AA7575}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20750" windowHeight="9320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seasonsExported" sheetId="1" r:id="rId1"/>
+    <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>mixed_1</t>
-  </si>
-  <si>
-    <t>mixed_2</t>
-  </si>
-  <si>
-    <t>spring_1</t>
-  </si>
-  <si>
-    <t>spring_2</t>
-  </si>
-  <si>
-    <t>strat_1</t>
-  </si>
-  <si>
-    <t>strat_2</t>
-  </si>
-  <si>
-    <t>fall_1</t>
-  </si>
-  <si>
-    <t>fall_2</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>from glider(s)</t>
   </si>
   <si>
-    <t>might want to shift all dates to one time step earlier</t>
-  </si>
-  <si>
-    <t>something wacky with DCM this year - set season manually</t>
-  </si>
-  <si>
     <t>something odd, use nominal dates</t>
   </si>
   <si>
@@ -71,6 +42,69 @@
   </si>
   <si>
     <t>use nominal dates for end spring/start strat</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Krista Longnecker</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>mixed_begin</t>
+  </si>
+  <si>
+    <t>mixed_end</t>
+  </si>
+  <si>
+    <t>spring_begin</t>
+  </si>
+  <si>
+    <t>spring_end</t>
+  </si>
+  <si>
+    <t>strat_begin</t>
+  </si>
+  <si>
+    <t>strat_end</t>
+  </si>
+  <si>
+    <t>fall_begin</t>
+  </si>
+  <si>
+    <t>fall_end</t>
+  </si>
+  <si>
+    <t>Seasons are as follows:</t>
+  </si>
+  <si>
+    <t>mixed = 1</t>
+  </si>
+  <si>
+    <t>spring = 2</t>
+  </si>
+  <si>
+    <t>stratified (summer) = 3</t>
+  </si>
+  <si>
+    <t>fall = 4</t>
+  </si>
+  <si>
+    <t>See Ruth's physical framework documentation for overview</t>
+  </si>
+  <si>
+    <t>See github.com/redbluewater/BATSallTime/ for the MATLAB code used to start the automated season definitions</t>
+  </si>
+  <si>
+    <t>After automation, I just manually tuned the dates for each transition with the end result in this Excel file</t>
+  </si>
+  <si>
+    <t>set seasons manually, fluorescence data are wacky</t>
   </si>
 </sst>
 </file>
@@ -213,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,18 +425,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -566,27 +588,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -950,135 +962,135 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="13.90625" style="1"/>
-    <col min="10" max="10" width="44" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="13.90625" style="1"/>
+    <col min="1" max="9" width="13.90625" style="5"/>
+    <col min="10" max="10" width="44" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="13.90625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1988</v>
+      </c>
+      <c r="C2" s="1">
+        <v>32234</v>
+      </c>
+      <c r="D2" s="1">
+        <v>32234</v>
+      </c>
+      <c r="E2" s="1">
+        <v>32253</v>
+      </c>
+      <c r="F2" s="1">
+        <v>32253</v>
+      </c>
+      <c r="G2" s="1">
+        <v>32448</v>
+      </c>
+      <c r="H2" s="1">
+        <v>32448</v>
+      </c>
+      <c r="I2" s="1">
+        <v>32492</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>1989</v>
+      </c>
+      <c r="B3" s="1">
+        <v>32492</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32599</v>
+      </c>
+      <c r="D3" s="1">
+        <v>32599</v>
+      </c>
+      <c r="E3" s="1">
+        <v>32678</v>
+      </c>
+      <c r="F3" s="1">
+        <v>32678</v>
+      </c>
+      <c r="G3" s="1">
+        <v>32830</v>
+      </c>
+      <c r="H3" s="1">
+        <v>32830</v>
+      </c>
+      <c r="I3" s="1">
+        <v>32860</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1988</v>
-      </c>
-      <c r="C2" s="2">
-        <v>32234</v>
-      </c>
-      <c r="D2" s="2">
-        <v>32234</v>
-      </c>
-      <c r="E2" s="2">
-        <v>32253</v>
-      </c>
-      <c r="F2" s="2">
-        <v>32253</v>
-      </c>
-      <c r="G2" s="2">
-        <v>32448</v>
-      </c>
-      <c r="H2" s="2">
-        <v>32448</v>
-      </c>
-      <c r="I2" s="2">
-        <v>32492</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>1989</v>
-      </c>
-      <c r="B3" s="2">
-        <v>32492</v>
-      </c>
-      <c r="C3" s="2">
-        <v>32599</v>
-      </c>
-      <c r="D3" s="2">
-        <v>32599</v>
-      </c>
-      <c r="E3" s="2">
-        <v>32678</v>
-      </c>
-      <c r="F3" s="2">
-        <v>32678</v>
-      </c>
-      <c r="G3" s="2">
-        <v>32830</v>
-      </c>
-      <c r="H3" s="2">
-        <v>32830</v>
-      </c>
-      <c r="I3" s="2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>1990</v>
+      </c>
+      <c r="B4" s="1">
         <v>32860</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>1990</v>
-      </c>
-      <c r="B4" s="2">
-        <v>32860</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>32964</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>32964</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>33044</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>33044</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>33181</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>33181</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>33209</v>
       </c>
     </row>
@@ -1086,1016 +1098,1092 @@
       <c r="A5" s="5">
         <v>1991</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>33209</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>33356</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>33356</v>
       </c>
-      <c r="E5" s="2">
-        <v>33373</v>
-      </c>
-      <c r="F5" s="2">
-        <v>33373</v>
-      </c>
-      <c r="G5" s="2">
-        <v>33519</v>
-      </c>
-      <c r="H5" s="2">
-        <v>33519</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="E5" s="1">
+        <v>33406</v>
+      </c>
+      <c r="F5" s="1">
+        <v>33406</v>
+      </c>
+      <c r="G5" s="1">
+        <v>33521</v>
+      </c>
+      <c r="H5" s="1">
+        <v>33521</v>
+      </c>
+      <c r="I5" s="1">
         <v>33580</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>1992</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>33580</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>33705</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>33705</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>33741</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>33741</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>33874</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>33874</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>33944</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>1993</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>33944</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>34060</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>34060</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>34079</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>34079</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>34274</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>34274</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>34318</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>13</v>
+      <c r="J7" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>1994</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>34318</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>34428</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>34428</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>34497</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>34497</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>34595</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>34595</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>34675</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>1995</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>34675</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>34798</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>34798</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>34815</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>34815</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>35013</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>35013</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>35046</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>1996</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>35046</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>35177</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>35177</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>35190</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>35190</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>35365</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>35365</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>35410</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>1997</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>35410</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>35554</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>35554</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>35590</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>35590</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>35708</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>35708</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>35772</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>1998</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>35772</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>35891</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>35891</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>35947</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>35947</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>36115</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>36115</v>
       </c>
-      <c r="I12" s="2">
-        <v>35807</v>
+      <c r="I12" s="1">
+        <v>36172</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>1999</v>
       </c>
-      <c r="B13" s="2">
-        <v>35807</v>
-      </c>
-      <c r="C13" s="2">
-        <v>36258</v>
-      </c>
-      <c r="D13" s="2">
-        <v>36258</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="B13" s="1">
+        <v>36172</v>
+      </c>
+      <c r="C13" s="1">
+        <v>36260</v>
+      </c>
+      <c r="D13" s="1">
+        <v>36260</v>
+      </c>
+      <c r="E13" s="1">
         <v>36283</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>36283</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>36417</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>36417</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>36502</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>16</v>
+      <c r="J13" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>2000</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>36502</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>36625</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>36625</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>36654</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>36654</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>36796</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>36796</v>
       </c>
-      <c r="I14" s="2">
-        <v>36552</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>12</v>
+      <c r="I14" s="1">
+        <v>36918</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>2001</v>
       </c>
-      <c r="B15" s="2">
-        <v>36552</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="1">
+        <v>36918</v>
+      </c>
+      <c r="C15" s="1">
         <v>36998</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>36998</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>37024</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>37024</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>37172</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>37172</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>37235</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>2002</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>37235</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>37360</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>37360</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>37388</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>37388</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>37535</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>37535</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>37598</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+      <c r="A17" s="5">
         <v>2003</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>37598</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>37712</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>37712</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>37732</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>37732</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>37910</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>37910</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>37956</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>2004</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>37956</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="1">
         <v>38096</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="1">
         <v>38096</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>38152</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>38152</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>38272</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>38272</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>38328</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>2005</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>38328</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>38460</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>38460</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="1">
         <v>38487</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="1">
         <v>38487</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="1">
         <v>38600</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="1">
         <v>38600</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>38693</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>2006</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>38693</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>38811</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>38811</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>38845</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>38845</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>38999</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>38999</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>39054</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>12</v>
+      <c r="J20" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>2007</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>39054</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>39185</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>39185</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>39216</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>39216</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>39330</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>39330</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>39420</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>2008</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>39420</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>39551</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>39551</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>39596</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>39596</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>39735</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>39735</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <v>39795</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>2009</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>39795</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="1">
         <v>39947</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="1">
         <v>39947</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="1">
         <v>39973</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="1">
         <v>39973</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>40065</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>40065</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>40154</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>2010</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>40154</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="1">
         <v>40309</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="1">
         <v>40309</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="1">
         <v>40349</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="1">
         <v>40349</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>40469</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>40469</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>40519</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>2011</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>40519</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>40639</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>40639</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>40659</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>40659</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>40813</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>40813</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>40884</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>2012</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>40884</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>40974</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>40974</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="1">
         <v>41025</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="1">
         <v>41025</v>
       </c>
-      <c r="G26" s="2">
-        <v>41162</v>
-      </c>
-      <c r="H26" s="2">
-        <v>41162</v>
-      </c>
-      <c r="I26" s="2">
+      <c r="G26" s="1">
+        <v>41179</v>
+      </c>
+      <c r="H26" s="1">
+        <v>41179</v>
+      </c>
+      <c r="I26" s="1">
         <v>41252</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>2013</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>41252</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>41386</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>41386</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>41408</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>41408</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>41591</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>41591</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <v>41616</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>2014</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>41616</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="1">
         <v>41757</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="1">
         <v>41757</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>41800</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>41800</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>41908</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>41908</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>41982</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+      <c r="A29" s="5">
         <v>2015</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>41982</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="1">
         <v>42116</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="1">
         <v>42116</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="1">
         <v>42134</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="1">
         <v>42134</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="1">
         <v>42335</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="1">
         <v>42335</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="1">
         <v>42353</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>2016</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="1">
         <v>42353</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>42461</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>42461</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>42480</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>42480</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>42675</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>42675</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>42696</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>2017</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42696</v>
+      </c>
+      <c r="C31" s="1">
+        <v>42835</v>
+      </c>
+      <c r="D31" s="1">
+        <v>42835</v>
+      </c>
+      <c r="E31" s="1">
+        <v>42851</v>
+      </c>
+      <c r="F31" s="1">
+        <v>42851</v>
+      </c>
+      <c r="G31" s="1">
+        <v>43009</v>
+      </c>
+      <c r="H31" s="1">
+        <v>43009</v>
+      </c>
+      <c r="I31" s="1">
+        <v>43101</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43195</v>
+      </c>
+      <c r="D32" s="1">
+        <v>43195</v>
+      </c>
+      <c r="E32" s="1">
+        <v>43216</v>
+      </c>
+      <c r="F32" s="1">
+        <v>43216</v>
+      </c>
+      <c r="G32" s="1">
+        <v>43405</v>
+      </c>
+      <c r="H32" s="1">
+        <v>43405</v>
+      </c>
+      <c r="I32" s="1">
+        <v>43449</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43449</v>
+      </c>
+      <c r="C33" s="1">
+        <v>43551</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43551</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43573</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43573</v>
+      </c>
+      <c r="G33" s="1">
+        <v>43775</v>
+      </c>
+      <c r="H33" s="1">
+        <v>43775</v>
+      </c>
+      <c r="I33" s="1">
+        <v>43805</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
+        <v>2020</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43805</v>
+      </c>
+      <c r="C34" s="1">
+        <v>43922</v>
+      </c>
+      <c r="D34" s="1">
+        <v>43922</v>
+      </c>
+      <c r="E34" s="1">
+        <v>43936</v>
+      </c>
+      <c r="F34" s="1">
+        <v>43936</v>
+      </c>
+      <c r="G34" s="1">
+        <v>44136</v>
+      </c>
+      <c r="H34" s="1">
+        <v>44136</v>
+      </c>
+      <c r="I34" s="1">
+        <v>44180</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <v>2021</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44180</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44287</v>
+      </c>
+      <c r="D35" s="1">
+        <v>44287</v>
+      </c>
+      <c r="E35" s="1">
+        <v>44311</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44311</v>
+      </c>
+      <c r="G35" s="1">
+        <v>44489</v>
+      </c>
+      <c r="H35" s="1">
+        <v>44489</v>
+      </c>
+      <c r="I35" s="1">
+        <v>44526</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
+        <v>2022</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44526</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44656</v>
+      </c>
+      <c r="D36" s="1">
+        <v>44656</v>
+      </c>
+      <c r="E36" s="1">
+        <v>44682</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44682</v>
+      </c>
+      <c r="G36" s="1">
+        <v>44866</v>
+      </c>
+      <c r="H36" s="1">
+        <v>44866</v>
+      </c>
+      <c r="I36" s="1">
+        <v>44910</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
+        <v>2023</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44910</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45017</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45017</v>
+      </c>
+      <c r="E37" s="1">
+        <v>45041</v>
+      </c>
+      <c r="F37" s="1">
+        <v>45041</v>
+      </c>
+      <c r="G37" s="1">
+        <v>45231</v>
+      </c>
+      <c r="H37" s="1">
+        <v>45231</v>
+      </c>
+      <c r="I37" s="1">
+        <v>45275</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45275</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45400</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45400</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45414</v>
+      </c>
+      <c r="F38" s="1">
+        <v>45414</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAAA878-EFC2-4D53-AF73-1CA7F3BE4D76}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B31" s="2">
-        <v>42696</v>
-      </c>
-      <c r="C31" s="2">
-        <v>42835</v>
-      </c>
-      <c r="D31" s="2">
-        <v>42835</v>
-      </c>
-      <c r="E31" s="2">
-        <v>42851</v>
-      </c>
-      <c r="F31" s="2">
-        <v>42851</v>
-      </c>
-      <c r="G31" s="2">
-        <v>43009</v>
-      </c>
-      <c r="H31" s="2">
-        <v>43009</v>
-      </c>
-      <c r="I31" s="2">
-        <v>43101</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B32" s="2">
-        <v>43101</v>
-      </c>
-      <c r="C32" s="2">
-        <v>43195</v>
-      </c>
-      <c r="D32" s="2">
-        <v>43195</v>
-      </c>
-      <c r="E32" s="2">
-        <v>43216</v>
-      </c>
-      <c r="F32" s="2">
-        <v>43216</v>
-      </c>
-      <c r="G32" s="2">
-        <v>43405</v>
-      </c>
-      <c r="H32" s="2">
-        <v>43405</v>
-      </c>
-      <c r="I32" s="2">
-        <v>43449</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B33" s="2">
-        <v>43449</v>
-      </c>
-      <c r="C33" s="2">
-        <v>43551</v>
-      </c>
-      <c r="D33" s="2">
-        <v>43551</v>
-      </c>
-      <c r="E33" s="2">
-        <v>43573</v>
-      </c>
-      <c r="F33" s="2">
-        <v>43573</v>
-      </c>
-      <c r="G33" s="2">
-        <v>43775</v>
-      </c>
-      <c r="H33" s="2">
-        <v>43775</v>
-      </c>
-      <c r="I33" s="2">
-        <v>43805</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>2020</v>
-      </c>
-      <c r="B34" s="2">
-        <v>43805</v>
-      </c>
-      <c r="C34" s="2">
-        <v>43922</v>
-      </c>
-      <c r="D34" s="2">
-        <v>43922</v>
-      </c>
-      <c r="E34" s="2">
-        <v>43936</v>
-      </c>
-      <c r="F34" s="2">
-        <v>43936</v>
-      </c>
-      <c r="G34" s="2">
-        <v>44136</v>
-      </c>
-      <c r="H34" s="2">
-        <v>44136</v>
-      </c>
-      <c r="I34" s="2">
-        <v>44180</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>2021</v>
-      </c>
-      <c r="B35" s="2">
-        <v>44180</v>
-      </c>
-      <c r="C35" s="2">
-        <v>44287</v>
-      </c>
-      <c r="D35" s="2">
-        <v>44287</v>
-      </c>
-      <c r="E35" s="2">
-        <v>44311</v>
-      </c>
-      <c r="F35" s="2">
-        <v>44311</v>
-      </c>
-      <c r="G35" s="2">
-        <v>44489</v>
-      </c>
-      <c r="H35" s="2">
-        <v>44489</v>
-      </c>
-      <c r="I35" s="2">
-        <v>44526</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B36" s="2">
-        <v>44526</v>
-      </c>
-      <c r="C36" s="2">
-        <v>44656</v>
-      </c>
-      <c r="D36" s="2">
-        <v>44656</v>
-      </c>
-      <c r="E36" s="2">
-        <v>44682</v>
-      </c>
-      <c r="F36" s="2">
-        <v>44682</v>
-      </c>
-      <c r="G36" s="2">
-        <v>44866</v>
-      </c>
-      <c r="H36" s="2">
-        <v>44866</v>
-      </c>
-      <c r="I36" s="2">
-        <v>44910</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B37" s="2">
-        <v>44910</v>
-      </c>
-      <c r="C37" s="2">
-        <v>45017</v>
-      </c>
-      <c r="D37" s="2">
-        <v>45017</v>
-      </c>
-      <c r="E37" s="2">
-        <v>45041</v>
-      </c>
-      <c r="F37" s="2">
-        <v>45041</v>
-      </c>
-      <c r="G37" s="2">
-        <v>45231</v>
-      </c>
-      <c r="H37" s="2">
-        <v>45231</v>
-      </c>
-      <c r="I37" s="2">
-        <v>45275</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>2024</v>
-      </c>
-      <c r="B38" s="2">
-        <v>45275</v>
-      </c>
-      <c r="C38" s="2">
-        <v>45400</v>
-      </c>
-      <c r="D38" s="2">
-        <v>45400</v>
-      </c>
-      <c r="E38" s="2">
-        <v>45414</v>
-      </c>
-      <c r="F38" s="2">
-        <v>45414</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>45478</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>